<commit_message>
added AFDW for part of 20211026 extras
</commit_message>
<xml_diff>
--- a/RAnalysis/Data/Survival_Size/20211026_lengths_dryweights_raw.xlsx
+++ b/RAnalysis/Data/Survival_Size/20211026_lengths_dryweights_raw.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samjg\Documents\Github_repositories\Airradians_OA\RAnalysis\Data\Survival_Size\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samuel.gurr\Documents\Github_repositories\Airradians_OA-foodsupply\RAnalysis\Data\Survival_Size\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C5728CF6-AF45-4202-BD86-EDDDAAA638E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="-110" windowWidth="18490" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="816" yWindow="-108" windowWidth="18492" windowHeight="12216"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="137">
   <si>
     <t>treatment</t>
   </si>
@@ -436,12 +435,21 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>AFDW</t>
+  </si>
+  <si>
+    <t>Ash weight (loss of ignition of tissue tin + dry shell and tissue)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmmm\ d\,\ yyyy"/>
   </numFmts>
@@ -535,7 +543,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -574,11 +582,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -793,41 +803,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q997"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
-      <selection activeCell="C191" sqref="C191"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.69921875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.1640625" customWidth="1"/>
-    <col min="3" max="8" width="7.6640625" customWidth="1"/>
-    <col min="9" max="9" width="9.9140625" customWidth="1"/>
+    <col min="2" max="2" width="9.19921875" customWidth="1"/>
+    <col min="3" max="8" width="7.69921875" customWidth="1"/>
+    <col min="9" max="9" width="9.8984375" customWidth="1"/>
     <col min="10" max="10" width="23.5" customWidth="1"/>
-    <col min="11" max="11" width="17.25" customWidth="1"/>
-    <col min="12" max="12" width="7.6640625" customWidth="1"/>
-    <col min="13" max="13" width="9.75" customWidth="1"/>
-    <col min="14" max="14" width="7.6640625" customWidth="1"/>
-    <col min="15" max="15" width="13.75" customWidth="1"/>
-    <col min="16" max="27" width="7.6640625" customWidth="1"/>
+    <col min="11" max="11" width="17.19921875" customWidth="1"/>
+    <col min="12" max="13" width="17.19921875" style="22" customWidth="1"/>
+    <col min="14" max="14" width="7.69921875" customWidth="1"/>
+    <col min="15" max="15" width="9.69921875" customWidth="1"/>
+    <col min="16" max="16" width="7.69921875" customWidth="1"/>
+    <col min="17" max="17" width="13.69921875" customWidth="1"/>
+    <col min="18" max="29" width="7.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="22">
-        <v>44495</v>
-      </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+    <row r="1" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="24">
+        <v>44495</v>
+      </c>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+    </row>
+    <row r="2" spans="1:21" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>133</v>
       </c>
@@ -861,16 +874,22 @@
       <c r="K2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="O2" s="7"/>
-      <c r="P2" s="8" t="s">
+      <c r="L2" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="S2" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="24">
+    <row r="3" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="23">
         <v>44495</v>
       </c>
       <c r="B3" s="2">
@@ -903,20 +922,26 @@
         <f>(J3/J4)*100</f>
         <v>7.8032786885245686</v>
       </c>
-      <c r="O3" s="11" t="s">
+      <c r="L3" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="M3" s="10"/>
+      <c r="Q3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="P3" s="12">
-        <f>AVERAGE(K3:K82,K160:L167)</f>
+      <c r="R3" s="12">
+        <f>AVERAGE(K3:K82,K160:N167)</f>
         <v>10.150046052861482</v>
       </c>
-      <c r="Q3" s="12">
+      <c r="S3" s="12">
         <f>AVERAGE(K83:K159,K168:K177)</f>
         <v>11.301900545888776</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="24">
+      <c r="T3" s="12"/>
+      <c r="U3" s="12"/>
+    </row>
+    <row r="4" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="23">
         <v>44495</v>
       </c>
       <c r="B4" s="2"/>
@@ -938,8 +963,8 @@
         <v>0.15249999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="24">
+    <row r="5" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="23">
         <v>44495</v>
       </c>
       <c r="B5" s="2">
@@ -972,20 +997,22 @@
         <f>(J5/J6)*100</f>
         <v>8.5667215815486575</v>
       </c>
-      <c r="O5" s="11" t="s">
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="Q5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="P5" s="12">
+      <c r="R5" s="12">
         <f>AVERAGE(E3:E82,E160:E167)</f>
         <v>9.5177083333333314</v>
       </c>
-      <c r="Q5" s="12">
+      <c r="S5" s="12">
         <f>AVERAGE(E83:E158,E168:E177)</f>
         <v>7.4716666666666649</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="24">
+    <row r="6" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="23">
         <v>44495</v>
       </c>
       <c r="B6" s="2"/>
@@ -1007,8 +1034,8 @@
         <v>6.0700000000000032E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="24">
+    <row r="7" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="23">
         <v>44495</v>
       </c>
       <c r="B7" s="2">
@@ -1041,9 +1068,11 @@
         <f>(J7/J8)*100</f>
         <v>7.1379071379071197</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="24">
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+    </row>
+    <row r="8" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="23">
         <v>44495</v>
       </c>
       <c r="B8" s="2"/>
@@ -1065,8 +1094,8 @@
         <v>0.14430000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="24">
+    <row r="9" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="23">
         <v>44495</v>
       </c>
       <c r="B9" s="2">
@@ -1099,9 +1128,11 @@
         <f>(J9/J10)*100</f>
         <v>8.9837997054492611</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="24">
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+    </row>
+    <row r="10" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="23">
         <v>44495</v>
       </c>
       <c r="B10" s="2"/>
@@ -1122,8 +1153,8 @@
         <v>6.7900000000000016E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="24">
+    <row r="11" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="23">
         <v>44495</v>
       </c>
       <c r="B11" s="2">
@@ -1156,9 +1187,11 @@
         <f>(J11/J12)*100</f>
         <v>10.57452123230645</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="24">
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+    </row>
+    <row r="12" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="23">
         <v>44495</v>
       </c>
       <c r="B12" s="2"/>
@@ -1180,8 +1213,8 @@
         <v>0.12009999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="24">
+    <row r="13" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="23">
         <v>44495</v>
       </c>
       <c r="B13" s="2">
@@ -1214,9 +1247,11 @@
         <f>(J13/J14)*100</f>
         <v>9.6622889305816404</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="24">
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+    </row>
+    <row r="14" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="23">
         <v>44495</v>
       </c>
       <c r="B14" s="2"/>
@@ -1238,8 +1273,8 @@
         <v>0.10660000000000003</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="24">
+    <row r="15" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="23">
         <v>44495</v>
       </c>
       <c r="B15" s="2">
@@ -1272,9 +1307,11 @@
         <f>(J15/J16)*100</f>
         <v>9.5785440613026864</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="24">
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+    </row>
+    <row r="16" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="23">
         <v>44495</v>
       </c>
       <c r="B16" s="2"/>
@@ -1296,8 +1333,8 @@
         <v>2.6100000000000012E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="24">
+    <row r="17" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="23">
         <v>44495</v>
       </c>
       <c r="B17" s="2">
@@ -1330,9 +1367,11 @@
         <f>(J17/J18)*100</f>
         <v>9.375000000000048</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="24">
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+    </row>
+    <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="23">
         <v>44495</v>
       </c>
       <c r="B18" s="2"/>
@@ -1354,8 +1393,8 @@
         <v>2.5600000000000012E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="24">
+    <row r="19" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="23">
         <v>44495</v>
       </c>
       <c r="B19" s="2">
@@ -1390,9 +1429,11 @@
         <f>(J19/J20)*100</f>
         <v>9.5588235294117716</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="24">
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+    </row>
+    <row r="20" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="23">
         <v>44495</v>
       </c>
       <c r="B20" s="2"/>
@@ -1416,8 +1457,8 @@
         <v>6.8000000000000005E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="24">
+    <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="23">
         <v>44495</v>
       </c>
       <c r="B21" s="2">
@@ -1452,9 +1493,11 @@
         <f>(J21/J22)*100</f>
         <v>9.1967871485944421</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="24">
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+    </row>
+    <row r="22" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="23">
         <v>44495</v>
       </c>
       <c r="B22" s="2"/>
@@ -1478,8 +1521,8 @@
         <v>2.4899999999999978E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="24">
+    <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="23">
         <v>44495</v>
       </c>
       <c r="B23" s="2">
@@ -1514,9 +1557,11 @@
         <f>(J23/J24)*100</f>
         <v>9.2592592592593359</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="24">
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+    </row>
+    <row r="24" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="23">
         <v>44495</v>
       </c>
       <c r="B24" s="2"/>
@@ -1540,8 +1585,8 @@
         <v>5.3999999999999604E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="24">
+    <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="23">
         <v>44495</v>
       </c>
       <c r="B25" s="2">
@@ -1576,9 +1621,11 @@
         <f>(J25/J26)*100</f>
         <v>10.342555994729937</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="24">
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+    </row>
+    <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="23">
         <v>44495</v>
       </c>
       <c r="B26" s="2"/>
@@ -1602,8 +1649,8 @@
         <v>0.15180000000000005</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="24">
+    <row r="27" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="23">
         <v>44495</v>
       </c>
       <c r="B27" s="2">
@@ -1638,9 +1685,11 @@
         <f>(J27/J28)*100</f>
         <v>9.0497737556561244</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="24">
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+    </row>
+    <row r="28" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="23">
         <v>44495</v>
       </c>
       <c r="B28" s="2"/>
@@ -1664,8 +1713,8 @@
         <v>4.4199999999999962E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="24">
+    <row r="29" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="23">
         <v>44495</v>
       </c>
       <c r="B29" s="2">
@@ -1700,9 +1749,11 @@
         <f>(J29/J30)*100</f>
         <v>10.548523206751065</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="24">
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+    </row>
+    <row r="30" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="23">
         <v>44495</v>
       </c>
       <c r="B30" s="2"/>
@@ -1726,8 +1777,8 @@
         <v>4.7399999999999998E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="24">
+    <row r="31" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="23">
         <v>44495</v>
       </c>
       <c r="B31" s="2">
@@ -1762,9 +1813,11 @@
         <f>(J31/J32)*100</f>
         <v>6.8965517241376508</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="24">
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
+    </row>
+    <row r="32" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="23">
         <v>44495</v>
       </c>
       <c r="B32" s="2"/>
@@ -1788,8 +1841,8 @@
         <v>1.1599999999999999E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="24">
+    <row r="33" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="23">
         <v>44495</v>
       </c>
       <c r="B33" s="2">
@@ -1824,9 +1877,11 @@
         <f>(J33/J34)*100</f>
         <v>6.0344827586209826</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="24">
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+    </row>
+    <row r="34" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="23">
         <v>44495</v>
       </c>
       <c r="B34" s="2"/>
@@ -1850,8 +1905,8 @@
         <v>1.1599999999999999E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="24">
+    <row r="35" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="23">
         <v>44495</v>
       </c>
       <c r="B35" s="2">
@@ -1886,9 +1941,11 @@
         <f>(J35/J36)*100</f>
         <v>18.749999999999783</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="24">
+      <c r="L35" s="10"/>
+      <c r="M35" s="10"/>
+    </row>
+    <row r="36" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="23">
         <v>44495</v>
       </c>
       <c r="B36" s="2"/>
@@ -1912,8 +1969,8 @@
         <v>6.3999999999999613E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="24">
+    <row r="37" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="23">
         <v>44495</v>
       </c>
       <c r="B37" s="2">
@@ -1948,9 +2005,11 @@
         <f>(J37/J38)*100</f>
         <v>9.3784078516902909</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="24">
+      <c r="L37" s="10"/>
+      <c r="M37" s="10"/>
+    </row>
+    <row r="38" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="23">
         <v>44495</v>
       </c>
       <c r="B38" s="2"/>
@@ -1974,8 +2033,8 @@
         <v>9.1700000000000004E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="24">
+    <row r="39" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="23">
         <v>44495</v>
       </c>
       <c r="B39" s="2">
@@ -2010,9 +2069,11 @@
         <f>(J39/J40)*100</f>
         <v>12.295081967213136</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="24">
+      <c r="L39" s="10"/>
+      <c r="M39" s="10"/>
+    </row>
+    <row r="40" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="23">
         <v>44495</v>
       </c>
       <c r="B40" s="2"/>
@@ -2036,8 +2097,8 @@
         <v>1.2199999999999989E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="24">
+    <row r="41" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="23">
         <v>44495</v>
       </c>
       <c r="B41" s="2">
@@ -2072,9 +2133,11 @@
         <f>(J41/J42)*100</f>
         <v>10.156250000000041</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="24">
+      <c r="L41" s="10"/>
+      <c r="M41" s="10"/>
+    </row>
+    <row r="42" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="23">
         <v>44495</v>
       </c>
       <c r="B42" s="2"/>
@@ -2098,8 +2161,8 @@
         <v>3.839999999999999E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="24">
+    <row r="43" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="23">
         <v>44495</v>
       </c>
       <c r="B43" s="2">
@@ -2134,9 +2197,11 @@
         <f>(J43/J44)*100</f>
         <v>11.154144074360941</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="24">
+      <c r="L43" s="10"/>
+      <c r="M43" s="10"/>
+    </row>
+    <row r="44" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="23">
         <v>44495</v>
       </c>
       <c r="B44" s="2"/>
@@ -2160,8 +2225,8 @@
         <v>0.12909999999999994</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="24">
+    <row r="45" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="23">
         <v>44495</v>
       </c>
       <c r="B45" s="2">
@@ -2196,9 +2261,11 @@
         <f>(J45/J46)*100</f>
         <v>11.533957845433248</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="24">
+      <c r="L45" s="10"/>
+      <c r="M45" s="10"/>
+    </row>
+    <row r="46" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="23">
         <v>44495</v>
       </c>
       <c r="B46" s="2">
@@ -2226,8 +2293,8 @@
         <v>0.17080000000000006</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="24">
+    <row r="47" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="23">
         <v>44495</v>
       </c>
       <c r="B47" s="2">
@@ -2262,9 +2329,11 @@
         <f>(J47/J48)*100</f>
         <v>10.180337405468272</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="24">
+      <c r="L47" s="10"/>
+      <c r="M47" s="10"/>
+    </row>
+    <row r="48" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="23">
         <v>44495</v>
       </c>
       <c r="B48" s="2">
@@ -2292,8 +2361,8 @@
         <v>0.1719</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="24">
+    <row r="49" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="23">
         <v>44495</v>
       </c>
       <c r="B49" s="2">
@@ -2328,9 +2397,11 @@
         <f>(J49/J50)*100</f>
         <v>10.594795539033422</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="24">
+      <c r="L49" s="10"/>
+      <c r="M49" s="10"/>
+    </row>
+    <row r="50" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="23">
         <v>44495</v>
       </c>
       <c r="B50" s="2">
@@ -2358,8 +2429,8 @@
         <v>0.10760000000000003</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="24">
+    <row r="51" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="23">
         <v>44495</v>
       </c>
       <c r="B51" s="2">
@@ -2394,9 +2465,11 @@
         <f>(J51/J52)*100</f>
         <v>10.294117647058547</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="24">
+      <c r="L51" s="10"/>
+      <c r="M51" s="10"/>
+    </row>
+    <row r="52" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="23">
         <v>44495</v>
       </c>
       <c r="B52" s="2">
@@ -2424,8 +2497,8 @@
         <v>6.7999999999999727E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="24">
+    <row r="53" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="23">
         <v>44495</v>
       </c>
       <c r="B53" s="2">
@@ -2450,12 +2523,12 @@
         <v>13</v>
       </c>
       <c r="I53" s="16"/>
-      <c r="L53" s="11" t="s">
+      <c r="N53" s="11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="24">
+    <row r="54" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="23">
         <v>44495</v>
       </c>
       <c r="B54" s="2">
@@ -2477,8 +2550,8 @@
       </c>
       <c r="I54" s="16"/>
     </row>
-    <row r="55" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="24">
+    <row r="55" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="23">
         <v>44495</v>
       </c>
       <c r="B55" s="2">
@@ -2504,8 +2577,8 @@
       </c>
       <c r="I55" s="16"/>
     </row>
-    <row r="56" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="24">
+    <row r="56" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="23">
         <v>44495</v>
       </c>
       <c r="B56" s="2">
@@ -2527,8 +2600,8 @@
       </c>
       <c r="I56" s="16"/>
     </row>
-    <row r="57" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="24">
+    <row r="57" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="23">
         <v>44495</v>
       </c>
       <c r="B57" s="2">
@@ -2554,8 +2627,8 @@
       </c>
       <c r="I57" s="16"/>
     </row>
-    <row r="58" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="24">
+    <row r="58" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="23">
         <v>44495</v>
       </c>
       <c r="B58" s="2">
@@ -2577,8 +2650,8 @@
       </c>
       <c r="I58" s="16"/>
     </row>
-    <row r="59" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="24">
+    <row r="59" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="23">
         <v>44495</v>
       </c>
       <c r="B59" s="2">
@@ -2604,8 +2677,8 @@
       </c>
       <c r="I59" s="16"/>
     </row>
-    <row r="60" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="24">
+    <row r="60" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="23">
         <v>44495</v>
       </c>
       <c r="B60" s="2">
@@ -2627,8 +2700,8 @@
       </c>
       <c r="I60" s="16"/>
     </row>
-    <row r="61" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="24">
+    <row r="61" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="23">
         <v>44495</v>
       </c>
       <c r="B61" s="2">
@@ -2654,8 +2727,8 @@
       </c>
       <c r="I61" s="16"/>
     </row>
-    <row r="62" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="24">
+    <row r="62" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="23">
         <v>44495</v>
       </c>
       <c r="B62" s="2">
@@ -2677,8 +2750,8 @@
       </c>
       <c r="I62" s="16"/>
     </row>
-    <row r="63" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="24">
+    <row r="63" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="23">
         <v>44495</v>
       </c>
       <c r="B63" s="2">
@@ -2713,9 +2786,16 @@
         <f>(J63/J64)*100</f>
         <v>11.442307692307709</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="24">
+      <c r="L63" s="10">
+        <v>0.52410000000000001</v>
+      </c>
+      <c r="M63" s="10">
+        <f>((I63)+(I64-G64))-L63</f>
+        <v>9.200000000000097E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="23">
         <v>44495</v>
       </c>
       <c r="B64" s="2">
@@ -2743,8 +2823,8 @@
         <v>0.10400000000000004</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="24">
+    <row r="65" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="23">
         <v>44495</v>
       </c>
       <c r="B65" s="2">
@@ -2779,9 +2859,16 @@
         <f>(J65/J66)*100</f>
         <v>11.296296296296287</v>
       </c>
-    </row>
-    <row r="66" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="24">
+      <c r="L65" s="10">
+        <v>0.52580000000000005</v>
+      </c>
+      <c r="M65" s="10">
+        <f>((I65)+(I66-G66))-L65</f>
+        <v>1.0299999999999976E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="23">
         <v>44495</v>
       </c>
       <c r="B66" s="2">
@@ -2809,8 +2896,8 @@
         <v>0.10799999999999998</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="24">
+    <row r="67" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="23">
         <v>44495</v>
       </c>
       <c r="B67" s="2">
@@ -2845,9 +2932,16 @@
         <f>(J67/J68)*100</f>
         <v>9.7222222222221752</v>
       </c>
-    </row>
-    <row r="68" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="24">
+      <c r="L67" s="10">
+        <v>0.4652</v>
+      </c>
+      <c r="M67" s="10">
+        <f>((I67)+(I68-G68))-L67</f>
+        <v>3.9000000000000146E-3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="23">
         <v>44495</v>
       </c>
       <c r="B68" s="2">
@@ -2875,8 +2969,8 @@
         <v>4.3200000000000016E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="24">
+    <row r="69" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="23">
         <v>44495</v>
       </c>
       <c r="B69" s="2">
@@ -2911,9 +3005,16 @@
         <f>(J69/J70)*100</f>
         <v>9.1863517060367617</v>
       </c>
-    </row>
-    <row r="70" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="24">
+      <c r="L69" s="10">
+        <v>0.44590000000000002</v>
+      </c>
+      <c r="M69" s="10">
+        <f>((I69)+(I70-G70))-L69</f>
+        <v>3.4999999999999476E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="23">
         <v>44495</v>
       </c>
       <c r="B70" s="2">
@@ -2941,8 +3042,8 @@
         <v>3.8099999999999967E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="24">
+    <row r="71" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="23">
         <v>44495</v>
       </c>
       <c r="B71" s="2">
@@ -2974,12 +3075,19 @@
         <v>2.9999999999996696E-4</v>
       </c>
       <c r="K71" s="17"/>
-      <c r="L71" s="11" t="s">
+      <c r="L71" s="17">
+        <v>0.44419999999999998</v>
+      </c>
+      <c r="M71" s="10">
+        <f>((I71)+(I72-G72))-L71</f>
+        <v>1.5000000000000013E-3</v>
+      </c>
+      <c r="N71" s="11" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="24">
+    <row r="72" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="23">
         <v>44495</v>
       </c>
       <c r="B72" s="2">
@@ -3007,8 +3115,8 @@
         <v>2.9700000000000004E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="24">
+    <row r="73" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="23">
         <v>44495</v>
       </c>
       <c r="B73" s="2">
@@ -3043,9 +3151,16 @@
         <f>(J73/J74)*100</f>
         <v>10.067114093959743</v>
       </c>
-    </row>
-    <row r="74" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="24">
+      <c r="L73" s="10">
+        <v>0.44259999999999999</v>
+      </c>
+      <c r="M73" s="10">
+        <f>((I73)+(I74-G74))-L73</f>
+        <v>3.0999999999999917E-3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="23">
         <v>44495</v>
       </c>
       <c r="B74" s="2">
@@ -3073,8 +3188,8 @@
         <v>2.9799999999999993E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="24">
+    <row r="75" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="23">
         <v>44495</v>
       </c>
       <c r="B75" s="2">
@@ -3109,9 +3224,16 @@
         <f>(J75/J76)*100</f>
         <v>9.0909090909090473</v>
       </c>
-    </row>
-    <row r="76" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="24">
+      <c r="L75" s="10">
+        <v>0.43790000000000001</v>
+      </c>
+      <c r="M75" s="10">
+        <f>((I75)+(I76-G76))-L75</f>
+        <v>2.6999999999999802E-3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="23">
         <v>44495</v>
       </c>
       <c r="B76" s="2">
@@ -3139,8 +3261,8 @@
         <v>2.3100000000000009E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="24">
+    <row r="77" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="23">
         <v>44495</v>
       </c>
       <c r="B77" s="2">
@@ -3175,9 +3297,16 @@
         <f>(J77/J78)*100</f>
         <v>9.0909090909090686</v>
       </c>
-    </row>
-    <row r="78" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="24">
+      <c r="L77" s="10">
+        <v>0.43419999999999997</v>
+      </c>
+      <c r="M77" s="10">
+        <f>((I77)+(I78-G78))-L77</f>
+        <v>2.2999999999999687E-3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="23">
         <v>44495</v>
       </c>
       <c r="B78" s="2">
@@ -3205,8 +3334,8 @@
         <v>2.3099999999999954E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="24">
+    <row r="79" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="23">
         <v>44495</v>
       </c>
       <c r="B79" s="2">
@@ -3241,9 +3370,16 @@
         <f>(J79/J80)*100</f>
         <v>6.4516129032257101</v>
       </c>
-    </row>
-    <row r="80" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="24">
+      <c r="L79" s="10">
+        <v>0.43070000000000003</v>
+      </c>
+      <c r="M79" s="10">
+        <f>((I79)+(I80-G80))-L79</f>
+        <v>5.9999999999993392E-4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="23">
         <v>44495</v>
       </c>
       <c r="B80" s="2">
@@ -3271,8 +3407,8 @@
         <v>9.299999999999975E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="24">
+    <row r="81" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="23">
         <v>44495</v>
       </c>
       <c r="B81" s="2">
@@ -3307,9 +3443,16 @@
         <f>(J81/J82)*100</f>
         <v>13.793103448276325</v>
       </c>
-    </row>
-    <row r="82" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="24">
+      <c r="L81" s="10">
+        <v>0.42559999999999998</v>
+      </c>
+      <c r="M81" s="10">
+        <f>((I81)+(I82-G82))-L81</f>
+        <v>5.0000000000000044E-4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="23">
         <v>44495</v>
       </c>
       <c r="B82" s="2">
@@ -3337,8 +3480,8 @@
         <v>5.7999999999999718E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="24">
+    <row r="83" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="23">
         <v>44495</v>
       </c>
       <c r="B83" s="2">
@@ -3373,9 +3516,16 @@
         <f>(J83/J84)*100</f>
         <v>10.769230769230878</v>
       </c>
-    </row>
-    <row r="84" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="24">
+      <c r="L83" s="10">
+        <v>0.43780000000000002</v>
+      </c>
+      <c r="M83" s="10">
+        <f>((I83)+(I84-G84))-L83</f>
+        <v>2.7999999999999692E-3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="23">
         <v>44495</v>
       </c>
       <c r="B84" s="2"/>
@@ -3399,8 +3549,8 @@
         <v>2.5999999999999968E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="24">
+    <row r="85" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="23">
         <v>44495</v>
       </c>
       <c r="B85" s="2">
@@ -3435,9 +3585,16 @@
         <f>(J85/J86)*100</f>
         <v>9.8181818181818183</v>
       </c>
-    </row>
-    <row r="86" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="24">
+      <c r="L85" s="10">
+        <v>0.49630000000000002</v>
+      </c>
+      <c r="M85" s="10">
+        <f>((I85)+(I86-G86))-L85</f>
+        <v>6.8999999999999617E-3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="23">
         <v>44495</v>
       </c>
       <c r="B86" s="2"/>
@@ -3461,8 +3618,8 @@
         <v>8.2499999999999962E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="24">
+    <row r="87" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="23">
         <v>44495</v>
       </c>
       <c r="B87" s="2">
@@ -3497,9 +3654,16 @@
         <f>(J87/J88)*100</f>
         <v>6.0606060606061112</v>
       </c>
-    </row>
-    <row r="88" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="24">
+      <c r="L87" s="10">
+        <v>0.434</v>
+      </c>
+      <c r="M87" s="10">
+        <f>((I87)+(I88-G88))-L87</f>
+        <v>1.7000000000000348E-3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="23">
         <v>44495</v>
       </c>
       <c r="B88" s="2"/>
@@ -3523,8 +3687,8 @@
         <v>2.3100000000000009E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="24">
+    <row r="89" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="23">
         <v>44495</v>
       </c>
       <c r="B89" s="2">
@@ -3559,9 +3723,16 @@
         <f>(J89/J90)*100</f>
         <v>17.948717948717999</v>
       </c>
-    </row>
-    <row r="90" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="24">
+      <c r="L89" s="10">
+        <v>0.43559999999999999</v>
+      </c>
+      <c r="M89" s="10">
+        <f>((I89)+(I90-G90))-L89</f>
+        <v>3.3999999999999586E-3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="23">
         <v>44495</v>
       </c>
       <c r="B90" s="2"/>
@@ -3585,8 +3756,8 @@
         <v>1.9499999999999962E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="24">
+    <row r="91" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="23">
         <v>44495</v>
       </c>
       <c r="B91" s="2">
@@ -3621,9 +3792,16 @@
         <f>(J91/J92)*100</f>
         <v>8.9303238469087312</v>
       </c>
-    </row>
-    <row r="92" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="24">
+      <c r="L91" s="10">
+        <v>0.51339999999999997</v>
+      </c>
+      <c r="M91" s="10">
+        <f>((I91)+(I92-G92))-L91</f>
+        <v>9.5999999999999419E-3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="23">
         <v>44495</v>
       </c>
       <c r="B92" s="2"/>
@@ -3647,8 +3825,8 @@
         <v>0.10189999999999999</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="24">
+    <row r="93" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="23">
         <v>44495</v>
       </c>
       <c r="B93" s="2">
@@ -3683,9 +3861,16 @@
         <f>(J93/J94)*100</f>
         <v>10.382513661201962</v>
       </c>
-    </row>
-    <row r="94" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A94" s="24">
+      <c r="L93" s="10">
+        <v>0.434</v>
+      </c>
+      <c r="M93" s="10">
+        <f>((I93)+(I94-G94))-L93</f>
+        <v>1.7999999999999683E-3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="23">
         <v>44495</v>
       </c>
       <c r="B94" s="2"/>
@@ -3709,8 +3894,8 @@
         <v>1.8299999999999983E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="24">
+    <row r="95" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="23">
         <v>44495</v>
       </c>
       <c r="B95" s="2">
@@ -3745,9 +3930,16 @@
         <f>(J95/J96)*100</f>
         <v>10.784313725490081</v>
       </c>
-    </row>
-    <row r="96" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="24">
+      <c r="L95" s="10">
+        <v>0.43440000000000001</v>
+      </c>
+      <c r="M95" s="10">
+        <f>((I95)+(I96-G96))-L95</f>
+        <v>2.3000000000000242E-3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="23">
         <v>44495</v>
       </c>
       <c r="B96" s="2"/>
@@ -3771,8 +3963,8 @@
         <v>2.0400000000000029E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="24">
+    <row r="97" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="23">
         <v>44495</v>
       </c>
       <c r="B97" s="2">
@@ -3807,9 +3999,16 @@
         <f>(J97/J98)*100</f>
         <v>12.121212121212478</v>
       </c>
-    </row>
-    <row r="98" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="24">
+      <c r="L97" s="10">
+        <v>0.4209</v>
+      </c>
+      <c r="M97" s="10">
+        <f>((I97)+(I98-G98))-L97</f>
+        <v>1.9000000000000128E-3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="23">
         <v>44495</v>
       </c>
       <c r="B98" s="2"/>
@@ -3833,8 +4032,8 @@
         <v>1.319999999999999E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="24">
+    <row r="99" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="23">
         <v>44495</v>
       </c>
       <c r="B99" s="2">
@@ -3869,9 +4068,16 @@
         <f>(J99/J100)*100</f>
         <v>8.4507042253522311</v>
       </c>
-    </row>
-    <row r="100" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="24">
+      <c r="L99" s="10">
+        <v>0.43509999999999999</v>
+      </c>
+      <c r="M99" s="10">
+        <f>((I99)+(I100-G100))-L99</f>
+        <v>1.9000000000000128E-3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="23">
         <v>44495</v>
       </c>
       <c r="B100" s="2"/>
@@ -3895,8 +4101,8 @@
         <v>2.1299999999999986E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="24">
+    <row r="101" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="23">
         <v>44495</v>
       </c>
       <c r="B101" s="2">
@@ -3931,9 +4137,16 @@
         <f>(J101/J102)*100</f>
         <v>22.033898305084715</v>
       </c>
-    </row>
-    <row r="102" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="24">
+      <c r="L101" s="10">
+        <v>0.42270000000000002</v>
+      </c>
+      <c r="M101" s="10">
+        <f>((I101)+(I102-G102))-L101</f>
+        <v>2.9999999999999472E-3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="23">
         <v>44495</v>
       </c>
       <c r="B102" s="2"/>
@@ -3957,8 +4170,8 @@
         <v>1.1799999999999977E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A103" s="24">
+    <row r="103" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="23">
         <v>44495</v>
       </c>
       <c r="B103" s="2">
@@ -3993,9 +4206,16 @@
         <f>(J103/J104)*100</f>
         <v>12.328767123287452</v>
       </c>
-    </row>
-    <row r="104" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A104" s="24">
+      <c r="L103" s="10">
+        <v>0.43280000000000002</v>
+      </c>
+      <c r="M103" s="10">
+        <f>((I103)+(I104-G104))-L103</f>
+        <v>1.2999999999999678E-3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="23">
         <v>44495</v>
       </c>
       <c r="B104" s="2"/>
@@ -4019,8 +4239,8 @@
         <v>1.4600000000000002E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="24">
+    <row r="105" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="23">
         <v>44495</v>
       </c>
       <c r="B105" s="2">
@@ -4055,9 +4275,16 @@
         <f>(J105/J106)*100</f>
         <v>9.7222222222222037</v>
       </c>
-    </row>
-    <row r="106" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="24">
+      <c r="L105" s="10">
+        <v>0.47589999999999999</v>
+      </c>
+      <c r="M105" s="10">
+        <f>((I105)+(I106-G106))-L105</f>
+        <v>3.6000000000000476E-3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="23">
         <v>44495</v>
       </c>
       <c r="B106" s="2"/>
@@ -4081,8 +4308,8 @@
         <v>5.760000000000004E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A107" s="24">
+    <row r="107" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="23">
         <v>44495</v>
       </c>
       <c r="B107" s="2">
@@ -4117,9 +4344,16 @@
         <f>(J107/J108)*100</f>
         <v>10.588235294117778</v>
       </c>
-    </row>
-    <row r="108" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A108" s="24">
+      <c r="L107" s="10">
+        <v>0.42920000000000003</v>
+      </c>
+      <c r="M107" s="10">
+        <f>((I107)+(I108-G108))-L107</f>
+        <v>5.9999999999998943E-4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="23">
         <v>44495</v>
       </c>
       <c r="B108" s="2"/>
@@ -4143,8 +4377,8 @@
         <v>8.5000000000000075E-3</v>
       </c>
     </row>
-    <row r="109" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A109" s="24">
+    <row r="109" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="23">
         <v>44495</v>
       </c>
       <c r="B109" s="2">
@@ -4179,9 +4413,16 @@
         <f>(J109/J110)*100</f>
         <v>12.182741116751339</v>
       </c>
-    </row>
-    <row r="110" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A110" s="24">
+      <c r="L109" s="10">
+        <v>0.43730000000000002</v>
+      </c>
+      <c r="M109" s="10">
+        <f>((I109)+(I110-G110))-L109</f>
+        <v>1.7999999999999683E-3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="23">
         <v>44495</v>
       </c>
       <c r="B110" s="2"/>
@@ -4205,8 +4446,8 @@
         <v>1.9699999999999995E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A111" s="24">
+    <row r="111" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="23">
         <v>44495</v>
       </c>
       <c r="B111" s="2">
@@ -4241,9 +4482,16 @@
         <f>(J111/J112)*100</f>
         <v>9.6385542168677443</v>
       </c>
-    </row>
-    <row r="112" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A112" s="24">
+      <c r="L111" s="10">
+        <v>0.42699999999999999</v>
+      </c>
+      <c r="M111" s="10">
+        <f>((I111)+(I112-G112))-L111</f>
+        <v>1.2000000000000344E-3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="23">
         <v>44495</v>
       </c>
       <c r="B112" s="2"/>
@@ -4267,8 +4515,8 @@
         <v>1.6600000000000004E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A113" s="24">
+    <row r="113" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="23">
         <v>44495</v>
       </c>
       <c r="B113" s="2">
@@ -4303,9 +4551,16 @@
         <f>(J113/J114)*100</f>
         <v>11.336032388664067</v>
       </c>
-    </row>
-    <row r="114" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A114" s="24">
+      <c r="L113" s="10">
+        <v>0.43709999999999999</v>
+      </c>
+      <c r="M113" s="10">
+        <f>((I113)+(I114-G114))-L113</f>
+        <v>1.3000000000000234E-3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="23">
         <v>44495</v>
       </c>
       <c r="B114" s="2"/>
@@ -4329,8 +4584,8 @@
         <v>2.47E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A115" s="24">
+    <row r="115" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="23">
         <v>44495</v>
       </c>
       <c r="B115" s="2">
@@ -4365,9 +4620,16 @@
         <f>(J115/J116)*100</f>
         <v>8.8235294117648344</v>
       </c>
-    </row>
-    <row r="116" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A116" s="24">
+      <c r="L115" s="10">
+        <v>0.42459999999999998</v>
+      </c>
+      <c r="M115" s="10">
+        <f>((I115)+(I116-G116))-L115</f>
+        <v>4.0000000000001146E-4</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="23">
         <v>44495</v>
       </c>
       <c r="B116" s="2"/>
@@ -4391,8 +4653,8 @@
         <v>1.0199999999999987E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A117" s="24">
+    <row r="117" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="23">
         <v>44495</v>
       </c>
       <c r="B117" s="2">
@@ -4427,9 +4689,16 @@
         <f>(J117/J118)*100</f>
         <v>12.643678160919364</v>
       </c>
-    </row>
-    <row r="118" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A118" s="24">
+      <c r="L117" s="10">
+        <v>0.41820000000000002</v>
+      </c>
+      <c r="M117" s="10">
+        <f>((I117)+(I118-G118))-L117</f>
+        <v>1.0000000000000009E-3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="23">
         <v>44495</v>
       </c>
       <c r="B118" s="2"/>
@@ -4453,8 +4722,8 @@
         <v>8.700000000000041E-3</v>
       </c>
     </row>
-    <row r="119" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A119" s="24">
+    <row r="119" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="23">
         <v>44495</v>
       </c>
       <c r="B119" s="2">
@@ -4489,9 +4758,11 @@
         <f>(J119/J120)*100</f>
         <v>12.499999999999918</v>
       </c>
-    </row>
-    <row r="120" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A120" s="24">
+      <c r="L119" s="10"/>
+      <c r="M119" s="10"/>
+    </row>
+    <row r="120" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="23">
         <v>44495</v>
       </c>
       <c r="B120" s="2">
@@ -4519,8 +4790,8 @@
         <v>2.5600000000000012E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A121" s="24">
+    <row r="121" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="23">
         <v>44495</v>
       </c>
       <c r="B121" s="2">
@@ -4555,9 +4826,11 @@
         <f>(J121/J122)*100</f>
         <v>12.578616352201271</v>
       </c>
-    </row>
-    <row r="122" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A122" s="24">
+      <c r="L121" s="10"/>
+      <c r="M121" s="10"/>
+    </row>
+    <row r="122" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="23">
         <v>44495</v>
       </c>
       <c r="B122" s="2">
@@ -4585,8 +4858,8 @@
         <v>3.1799999999999995E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A123" s="24">
+    <row r="123" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="23">
         <v>44495</v>
       </c>
       <c r="B123" s="2">
@@ -4621,9 +4894,11 @@
         <f>(J123/J124)*100</f>
         <v>12.499999999999844</v>
       </c>
-    </row>
-    <row r="124" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A124" s="24">
+      <c r="L123" s="10"/>
+      <c r="M123" s="10"/>
+    </row>
+    <row r="124" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="23">
         <v>44495</v>
       </c>
       <c r="B124" s="2">
@@ -4651,8 +4926,8 @@
         <v>2.2400000000000031E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A125" s="24">
+    <row r="125" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="23">
         <v>44495</v>
       </c>
       <c r="B125" s="2">
@@ -4687,9 +4962,11 @@
         <f>(J125/J126)*100</f>
         <v>12.258064516129103</v>
       </c>
-    </row>
-    <row r="126" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A126" s="24">
+      <c r="L125" s="10"/>
+      <c r="M125" s="10"/>
+    </row>
+    <row r="126" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A126" s="23">
         <v>44495</v>
       </c>
       <c r="B126" s="2">
@@ -4717,8 +4994,8 @@
         <v>1.5500000000000014E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A127" s="24">
+    <row r="127" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="23">
         <v>44495</v>
       </c>
       <c r="B127" s="2">
@@ -4753,9 +5030,11 @@
         <f>(J127/J128)*100</f>
         <v>13.793103448275779</v>
       </c>
-    </row>
-    <row r="128" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A128" s="24">
+      <c r="L127" s="10"/>
+      <c r="M127" s="10"/>
+    </row>
+    <row r="128" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="23">
         <v>44495</v>
       </c>
       <c r="B128" s="2">
@@ -4783,8 +5062,8 @@
         <v>1.1599999999999999E-2</v>
       </c>
     </row>
-    <row r="129" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A129" s="24">
+    <row r="129" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="23">
         <v>44495</v>
       </c>
       <c r="B129" s="2">
@@ -4819,9 +5098,11 @@
         <f>(J129/J130)*100</f>
         <v>8.1300813008130124</v>
       </c>
-    </row>
-    <row r="130" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A130" s="24">
+      <c r="L129" s="10"/>
+      <c r="M129" s="10"/>
+    </row>
+    <row r="130" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="23">
         <v>44495</v>
       </c>
       <c r="B130" s="2">
@@ -4849,8 +5130,8 @@
         <v>2.4600000000000011E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A131" s="24">
+    <row r="131" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="23">
         <v>44495</v>
       </c>
       <c r="B131" s="2">
@@ -4885,9 +5166,11 @@
         <f>(J131/J132)*100</f>
         <v>10.843373493975809</v>
       </c>
-    </row>
-    <row r="132" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A132" s="24">
+      <c r="L131" s="10"/>
+      <c r="M131" s="10"/>
+    </row>
+    <row r="132" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="23">
         <v>44495</v>
       </c>
       <c r="B132" s="2">
@@ -4915,8 +5198,8 @@
         <v>2.4900000000000033E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A133" s="24">
+    <row r="133" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="23">
         <v>44495</v>
       </c>
       <c r="B133" s="2">
@@ -4951,9 +5234,11 @@
         <f>(J133/J134)*100</f>
         <v>12.1661721068249</v>
       </c>
-    </row>
-    <row r="134" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A134" s="24">
+      <c r="L133" s="10"/>
+      <c r="M133" s="10"/>
+    </row>
+    <row r="134" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="23">
         <v>44495</v>
       </c>
       <c r="B134" s="2">
@@ -4981,8 +5266,8 @@
         <v>3.3700000000000008E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A135" s="24">
+    <row r="135" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A135" s="23">
         <v>44495</v>
       </c>
       <c r="B135" s="2">
@@ -5017,9 +5302,11 @@
         <f>(J135/J136)*100</f>
         <v>6.1349693251533655</v>
       </c>
-    </row>
-    <row r="136" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A136" s="24">
+      <c r="L135" s="10"/>
+      <c r="M135" s="10"/>
+    </row>
+    <row r="136" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="23">
         <v>44495</v>
       </c>
       <c r="B136" s="2">
@@ -5047,8 +5334,8 @@
         <v>1.6300000000000037E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A137" s="24">
+    <row r="137" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A137" s="23">
         <v>44495</v>
       </c>
       <c r="B137" s="2">
@@ -5083,9 +5370,11 @@
         <f>(J137/J138)*100</f>
         <v>15.555555555555472</v>
       </c>
-    </row>
-    <row r="138" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A138" s="24">
+      <c r="L137" s="10"/>
+      <c r="M137" s="10"/>
+    </row>
+    <row r="138" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A138" s="23">
         <v>44495</v>
       </c>
       <c r="B138" s="2">
@@ -5113,8 +5402,8 @@
         <v>1.3500000000000012E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A139" s="24">
+    <row r="139" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A139" s="23">
         <v>44495</v>
       </c>
       <c r="B139" s="2">
@@ -5146,12 +5435,19 @@
         <v>1.0999999999999899E-3</v>
       </c>
       <c r="K139" s="17"/>
-      <c r="L139" s="11" t="s">
+      <c r="L139" s="17">
+        <v>0.432</v>
+      </c>
+      <c r="M139" s="10">
+        <f>((I139)+(I140-G140))-L139</f>
+        <v>-6.0000000000000053E-3</v>
+      </c>
+      <c r="N139" s="11" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="140" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A140" s="24">
+    <row r="140" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A140" s="23">
         <v>44495</v>
       </c>
       <c r="B140" s="2">
@@ -5179,8 +5475,8 @@
         <v>4.0999999999999925E-3</v>
       </c>
     </row>
-    <row r="141" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A141" s="24">
+    <row r="141" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A141" s="23">
         <v>44495</v>
       </c>
       <c r="B141" s="2">
@@ -5215,9 +5511,16 @@
         <f>(J141/J142)*100</f>
         <v>9.3478260869565819</v>
       </c>
-    </row>
-    <row r="142" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A142" s="24">
+      <c r="L141" s="10">
+        <v>0.62460000000000004</v>
+      </c>
+      <c r="M141" s="10">
+        <f>((I141)+(I142-G142))-L141</f>
+        <v>-0.15420000000000006</v>
+      </c>
+    </row>
+    <row r="142" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A142" s="23">
         <v>44495</v>
       </c>
       <c r="B142" s="2">
@@ -5245,8 +5548,8 @@
         <v>4.5999999999999985E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A143" s="24">
+    <row r="143" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A143" s="23">
         <v>44495</v>
       </c>
       <c r="B143" s="2">
@@ -5281,9 +5584,16 @@
         <f>(J143/J144)*100</f>
         <v>12.753623188405831</v>
       </c>
-    </row>
-    <row r="144" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A144" s="24">
+      <c r="L143" s="10">
+        <v>0.4526</v>
+      </c>
+      <c r="M143" s="10">
+        <f>((I143)+(I144-G144))-L143</f>
+        <v>4.200000000000037E-3</v>
+      </c>
+    </row>
+    <row r="144" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A144" s="23">
         <v>44495</v>
       </c>
       <c r="B144" s="2">
@@ -5311,8 +5621,8 @@
         <v>3.4500000000000031E-2</v>
       </c>
     </row>
-    <row r="145" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A145" s="24">
+    <row r="145" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A145" s="23">
         <v>44495</v>
       </c>
       <c r="B145" s="2">
@@ -5344,12 +5654,19 @@
         <v>1.0999999999999899E-3</v>
       </c>
       <c r="K145" s="17"/>
-      <c r="L145" s="11" t="s">
+      <c r="L145" s="17">
+        <v>0.42970000000000003</v>
+      </c>
+      <c r="M145" s="10">
+        <f>((I145)+(I146-G146))-L145</f>
+        <v>2.2999999999999687E-3</v>
+      </c>
+      <c r="N145" s="11" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="146" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A146" s="24">
+    <row r="146" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A146" s="23">
         <v>44495</v>
       </c>
       <c r="B146" s="2">
@@ -5377,8 +5694,8 @@
         <v>1.1599999999999999E-2</v>
       </c>
     </row>
-    <row r="147" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A147" s="24">
+    <row r="147" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A147" s="23">
         <v>44495</v>
       </c>
       <c r="B147" s="2">
@@ -5413,9 +5730,16 @@
         <f>(J147/J148)*100</f>
         <v>13.0641330166271</v>
       </c>
-    </row>
-    <row r="148" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A148" s="24">
+      <c r="L147" s="10">
+        <v>0.45639999999999997</v>
+      </c>
+      <c r="M147" s="10">
+        <f>((I147)+(I148-G148))-L147</f>
+        <v>4.699999999999982E-3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A148" s="23">
         <v>44495</v>
       </c>
       <c r="B148" s="2">
@@ -5443,8 +5767,8 @@
         <v>4.2099999999999971E-2</v>
       </c>
     </row>
-    <row r="149" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A149" s="24">
+    <row r="149" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A149" s="23">
         <v>44495</v>
       </c>
       <c r="B149" s="2">
@@ -5479,9 +5803,16 @@
         <f>(J149/J150)*100</f>
         <v>11.598746081504823</v>
       </c>
-    </row>
-    <row r="150" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A150" s="24">
+      <c r="L149" s="10">
+        <v>0.44019999999999998</v>
+      </c>
+      <c r="M149" s="10">
+        <f>((I149)+(I150-G150))-L149</f>
+        <v>2.9000000000000137E-3</v>
+      </c>
+    </row>
+    <row r="150" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A150" s="23">
         <v>44495</v>
       </c>
       <c r="B150" s="2">
@@ -5509,8 +5840,8 @@
         <v>3.1899999999999984E-2</v>
       </c>
     </row>
-    <row r="151" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A151" s="24">
+    <row r="151" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A151" s="23">
         <v>44495</v>
       </c>
       <c r="B151" s="2">
@@ -5545,9 +5876,16 @@
         <f>(J151/J152)*100</f>
         <v>10.191082802547678</v>
       </c>
-    </row>
-    <row r="152" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A152" s="24">
+      <c r="L151" s="10">
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="M151" s="10">
+        <f>((I151)+(I152-G152))-L151</f>
+        <v>1.7000000000000348E-3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A152" s="23">
         <v>44495</v>
       </c>
       <c r="B152" s="2">
@@ -5575,8 +5913,8 @@
         <v>1.5700000000000047E-2</v>
       </c>
     </row>
-    <row r="153" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A153" s="24">
+    <row r="153" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A153" s="23">
         <v>44495</v>
       </c>
       <c r="B153" s="2">
@@ -5611,9 +5949,16 @@
         <f>(J153/J154)*100</f>
         <v>10.460251046025123</v>
       </c>
-    </row>
-    <row r="154" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A154" s="24">
+      <c r="L153" s="10">
+        <v>0.4345</v>
+      </c>
+      <c r="M153" s="10">
+        <f>((I153)+(I154-G154))-L153</f>
+        <v>2.2999999999999687E-3</v>
+      </c>
+    </row>
+    <row r="154" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A154" s="23">
         <v>44495</v>
       </c>
       <c r="B154" s="2">
@@ -5641,8 +5986,8 @@
         <v>2.3899999999999977E-2</v>
       </c>
     </row>
-    <row r="155" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A155" s="24">
+    <row r="155" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A155" s="23">
         <v>44495</v>
       </c>
       <c r="B155" s="2">
@@ -5677,9 +6022,16 @@
         <f>(J155/J156)*100</f>
         <v>10.404624277456636</v>
       </c>
-    </row>
-    <row r="156" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A156" s="24">
+      <c r="L155" s="10">
+        <v>0.44579999999999997</v>
+      </c>
+      <c r="M155" s="10">
+        <f>((I155)+(I156-G156))-L155</f>
+        <v>3.6999999999999811E-3</v>
+      </c>
+    </row>
+    <row r="156" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A156" s="23">
         <v>44495</v>
       </c>
       <c r="B156" s="2">
@@ -5707,8 +6059,8 @@
         <v>3.4599999999999964E-2</v>
       </c>
     </row>
-    <row r="157" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A157" s="24">
+    <row r="157" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A157" s="23">
         <v>44495</v>
       </c>
       <c r="B157" s="2">
@@ -5743,9 +6095,16 @@
         <f>(J157/J158)*100</f>
         <v>12.365591397849588</v>
       </c>
-    </row>
-    <row r="158" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A158" s="24">
+      <c r="L157" s="10">
+        <v>0.43419999999999997</v>
+      </c>
+      <c r="M157" s="10">
+        <f>((I157)+(I158-G158))-L157</f>
+        <v>2.1000000000000463E-3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A158" s="23">
         <v>44495</v>
       </c>
       <c r="B158" s="2">
@@ -5773,8 +6132,8 @@
         <v>1.8600000000000005E-2</v>
       </c>
     </row>
-    <row r="159" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A159" s="24">
+    <row r="159" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A159" s="23">
         <v>44495</v>
       </c>
       <c r="B159" s="2"/>
@@ -5785,12 +6144,15 @@
       <c r="G159" s="2"/>
       <c r="H159" s="2"/>
       <c r="I159" s="2"/>
-      <c r="L159" s="11" t="s">
+      <c r="L159" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="N159" s="11" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="160" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A160" s="24">
+    <row r="160" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A160" s="23">
         <v>44495</v>
       </c>
       <c r="B160" s="18">
@@ -5814,9 +6176,11 @@
       <c r="K160" s="21">
         <v>9.2841956060000008</v>
       </c>
-    </row>
-    <row r="161" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A161" s="24">
+      <c r="L160" s="21"/>
+      <c r="M160" s="21"/>
+    </row>
+    <row r="161" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A161" s="23">
         <v>44495</v>
       </c>
       <c r="B161" s="18">
@@ -5840,9 +6204,11 @@
       <c r="K161" s="21">
         <v>14.345114349999999</v>
       </c>
-    </row>
-    <row r="162" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A162" s="24">
+      <c r="L161" s="21"/>
+      <c r="M161" s="21"/>
+    </row>
+    <row r="162" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A162" s="23">
         <v>44495</v>
       </c>
       <c r="B162" s="18">
@@ -5866,9 +6232,11 @@
       <c r="K162" s="21">
         <v>10.777777779999999</v>
       </c>
-    </row>
-    <row r="163" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A163" s="24">
+      <c r="L162" s="21"/>
+      <c r="M162" s="21"/>
+    </row>
+    <row r="163" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A163" s="23">
         <v>44495</v>
       </c>
       <c r="B163" s="18">
@@ -5892,9 +6260,11 @@
       <c r="K163" s="21">
         <v>8.6560364459999999</v>
       </c>
-    </row>
-    <row r="164" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A164" s="24">
+      <c r="L163" s="21"/>
+      <c r="M163" s="21"/>
+    </row>
+    <row r="164" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A164" s="23">
         <v>44495</v>
       </c>
       <c r="B164" s="18">
@@ -5918,9 +6288,11 @@
       <c r="K164" s="21">
         <v>9.2807424590000007</v>
       </c>
-    </row>
-    <row r="165" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A165" s="24">
+      <c r="L164" s="21"/>
+      <c r="M164" s="21"/>
+    </row>
+    <row r="165" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A165" s="23">
         <v>44495</v>
       </c>
       <c r="B165" s="18">
@@ -5944,9 +6316,11 @@
       <c r="K165" s="21">
         <v>15.60283688</v>
       </c>
-    </row>
-    <row r="166" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A166" s="24">
+      <c r="L165" s="21"/>
+      <c r="M165" s="21"/>
+    </row>
+    <row r="166" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A166" s="23">
         <v>44495</v>
       </c>
       <c r="B166" s="18">
@@ -5970,9 +6344,11 @@
       <c r="K166" s="21">
         <v>10.7599699</v>
       </c>
-    </row>
-    <row r="167" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A167" s="24">
+      <c r="L166" s="21"/>
+      <c r="M166" s="21"/>
+    </row>
+    <row r="167" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A167" s="23">
         <v>44495</v>
       </c>
       <c r="B167" s="18">
@@ -5996,9 +6372,11 @@
       <c r="K167" s="21">
         <v>10.548523210000001</v>
       </c>
-    </row>
-    <row r="168" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A168" s="24">
+      <c r="L167" s="21"/>
+      <c r="M167" s="21"/>
+    </row>
+    <row r="168" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A168" s="23">
         <v>44495</v>
       </c>
       <c r="B168" s="18">
@@ -6022,9 +6400,11 @@
       <c r="K168" s="21">
         <v>8.8659793810000007</v>
       </c>
-    </row>
-    <row r="169" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A169" s="24">
+      <c r="L168" s="21"/>
+      <c r="M168" s="21"/>
+    </row>
+    <row r="169" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A169" s="23">
         <v>44495</v>
       </c>
       <c r="B169" s="18">
@@ -6048,9 +6428,11 @@
       <c r="K169" s="21">
         <v>11.27819549</v>
       </c>
-    </row>
-    <row r="170" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A170" s="24">
+      <c r="L169" s="21"/>
+      <c r="M169" s="21"/>
+    </row>
+    <row r="170" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A170" s="23">
         <v>44495</v>
       </c>
       <c r="B170" s="18">
@@ -6074,9 +6456,11 @@
       <c r="K170" s="21">
         <v>11.02941176</v>
       </c>
-    </row>
-    <row r="171" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A171" s="24">
+      <c r="L170" s="21"/>
+      <c r="M170" s="21"/>
+    </row>
+    <row r="171" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A171" s="23">
         <v>44495</v>
       </c>
       <c r="B171" s="18">
@@ -6100,9 +6484,11 @@
       <c r="K171" s="21">
         <v>8.7272727270000008</v>
       </c>
-    </row>
-    <row r="172" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A172" s="24">
+      <c r="L171" s="21"/>
+      <c r="M171" s="21"/>
+    </row>
+    <row r="172" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A172" s="23">
         <v>44495</v>
       </c>
       <c r="B172" s="18">
@@ -6126,9 +6512,11 @@
       <c r="K172" s="21">
         <v>10.43034282</v>
       </c>
-    </row>
-    <row r="173" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A173" s="24">
+      <c r="L172" s="21"/>
+      <c r="M172" s="21"/>
+    </row>
+    <row r="173" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A173" s="23">
         <v>44495</v>
       </c>
       <c r="B173" s="18">
@@ -6152,9 +6540,11 @@
       <c r="K173" s="21">
         <v>10.740203190000001</v>
       </c>
-    </row>
-    <row r="174" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A174" s="24">
+      <c r="L173" s="21"/>
+      <c r="M173" s="21"/>
+    </row>
+    <row r="174" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A174" s="23">
         <v>44495</v>
       </c>
       <c r="B174" s="18">
@@ -6178,9 +6568,11 @@
       <c r="K174" s="21">
         <v>12.998266900000001</v>
       </c>
-    </row>
-    <row r="175" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A175" s="24">
+      <c r="L174" s="21"/>
+      <c r="M174" s="21"/>
+    </row>
+    <row r="175" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A175" s="23">
         <v>44495</v>
       </c>
       <c r="B175" s="18">
@@ -6204,9 +6596,11 @@
       <c r="K175" s="21">
         <v>12.64916468</v>
       </c>
-    </row>
-    <row r="176" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A176" s="24">
+      <c r="L175" s="21"/>
+      <c r="M175" s="21"/>
+    </row>
+    <row r="176" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A176" s="23">
         <v>44495</v>
       </c>
       <c r="B176" s="18">
@@ -6230,9 +6624,11 @@
       <c r="K176" s="21">
         <v>11.187607570000001</v>
       </c>
-    </row>
-    <row r="177" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A177" s="24">
+      <c r="L176" s="21"/>
+      <c r="M176" s="21"/>
+    </row>
+    <row r="177" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A177" s="23">
         <v>44495</v>
       </c>
       <c r="B177" s="18">
@@ -6256,9 +6652,11 @@
       <c r="K177" s="21">
         <v>10.77170418</v>
       </c>
-    </row>
-    <row r="178" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A178" s="24">
+      <c r="L177" s="21"/>
+      <c r="M177" s="21"/>
+    </row>
+    <row r="178" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A178" s="23">
         <v>44495</v>
       </c>
       <c r="B178" s="18">
@@ -6277,8 +6675,8 @@
         <v>0.1411</v>
       </c>
     </row>
-    <row r="179" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A179" s="24">
+    <row r="179" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A179" s="23">
         <v>44495</v>
       </c>
       <c r="B179" s="18">
@@ -6297,8 +6695,8 @@
         <v>4.8099999999999997E-2</v>
       </c>
     </row>
-    <row r="180" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A180" s="24">
+    <row r="180" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A180" s="23">
         <v>44495</v>
       </c>
       <c r="B180" s="18">
@@ -6317,8 +6715,8 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="181" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A181" s="24">
+    <row r="181" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A181" s="23">
         <v>44495</v>
       </c>
       <c r="B181" s="18">
@@ -6337,8 +6735,8 @@
         <v>4.3900000000000002E-2</v>
       </c>
     </row>
-    <row r="182" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A182" s="24">
+    <row r="182" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A182" s="23">
         <v>44495</v>
       </c>
       <c r="B182" s="18">
@@ -6357,8 +6755,8 @@
         <v>0.1724</v>
       </c>
     </row>
-    <row r="183" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A183" s="24">
+    <row r="183" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A183" s="23">
         <v>44495</v>
       </c>
       <c r="B183" s="18">
@@ -6377,8 +6775,8 @@
         <v>8.4599999999999995E-2</v>
       </c>
     </row>
-    <row r="184" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A184" s="24">
+    <row r="184" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A184" s="23">
         <v>44495</v>
       </c>
       <c r="B184" s="18">
@@ -6397,8 +6795,8 @@
         <v>0.13289999999999999</v>
       </c>
     </row>
-    <row r="185" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A185" s="24">
+    <row r="185" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A185" s="23">
         <v>44495</v>
       </c>
       <c r="B185" s="18">
@@ -6417,8 +6815,8 @@
         <v>9.4799999999999995E-2</v>
       </c>
     </row>
-    <row r="186" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A186" s="24">
+    <row r="186" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A186" s="23">
         <v>44495</v>
       </c>
       <c r="B186" s="18">
@@ -6437,8 +6835,8 @@
         <v>4.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="187" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A187" s="24">
+    <row r="187" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A187" s="23">
         <v>44495</v>
       </c>
       <c r="B187" s="18">
@@ -6457,8 +6855,8 @@
         <v>2.6599999999999999E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A188" s="24">
+    <row r="188" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A188" s="23">
         <v>44495</v>
       </c>
       <c r="B188" s="18">
@@ -6477,8 +6875,8 @@
         <v>2.7199999999999998E-2</v>
       </c>
     </row>
-    <row r="189" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A189" s="24">
+    <row r="189" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A189" s="23">
         <v>44495</v>
       </c>
       <c r="B189" s="18">
@@ -6497,8 +6895,8 @@
         <v>2.75E-2</v>
       </c>
     </row>
-    <row r="190" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A190" s="24">
+    <row r="190" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A190" s="23">
         <v>44495</v>
       </c>
       <c r="B190" s="18">
@@ -6517,8 +6915,8 @@
         <v>0.1371</v>
       </c>
     </row>
-    <row r="191" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A191" s="24">
+    <row r="191" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A191" s="23">
         <v>44495</v>
       </c>
       <c r="B191" s="18">
@@ -6537,8 +6935,8 @@
         <v>6.8900000000000003E-2</v>
       </c>
     </row>
-    <row r="192" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A192" s="24">
+    <row r="192" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A192" s="23">
         <v>44495</v>
       </c>
       <c r="B192" s="18">
@@ -6557,8 +6955,8 @@
         <v>5.7700000000000001E-2</v>
       </c>
     </row>
-    <row r="193" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A193" s="24">
+    <row r="193" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A193" s="23">
         <v>44495</v>
       </c>
       <c r="B193" s="18">
@@ -6577,8 +6975,8 @@
         <v>4.19E-2</v>
       </c>
     </row>
-    <row r="194" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A194" s="24">
+    <row r="194" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A194" s="23">
         <v>44495</v>
       </c>
       <c r="B194" s="18">
@@ -6597,8 +6995,8 @@
         <v>5.8099999999999999E-2</v>
       </c>
     </row>
-    <row r="195" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A195" s="24">
+    <row r="195" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A195" s="23">
         <v>44495</v>
       </c>
       <c r="B195" s="18">
@@ -6617,808 +7015,808 @@
         <v>6.2199999999999998E-2</v>
       </c>
     </row>
-    <row r="196" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="197" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="198" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="199" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="200" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="201" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="202" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="203" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="204" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="205" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="206" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="207" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="208" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="196" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:D1"/>

</xml_diff>